<commit_message>
On change map ep00~ep04까지 세팅 완
전체 돌아보면서 일부 작업 더 필요한 것들 체크해서 공유 엑셀에다 올림
</commit_message>
<xml_diff>
--- a/Excel2Json/bin/ep03/ep03_1.xlsx
+++ b/Excel2Json/bin/ep03/ep03_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justb\GitHub\Slanted_Structure\Excel2Json\bin\ep03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D84EDA3-B5A3-4F6F-BE77-561BF39A007A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F565AB-7532-4BD9-A3E1-F034F68866DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="722" firstSheet="14" activeTab="18" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="301010" sheetId="2" r:id="rId1"/>
@@ -5635,8 +5635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B735065-E9DF-44C9-8F27-0ECDE1230632}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -6024,7 +6024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1233C3-FC6F-45A3-BAB7-B7B72BA8A977}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>

</xml_diff>